<commit_message>
[ADD] production robustness analysis
</commit_message>
<xml_diff>
--- a/environmental_conditions/wild_type_conditions.xlsx
+++ b/environmental_conditions/wild_type_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Pycharm_projects/lab_models/environmental_conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="212" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{09E343B3-98F3-4F2B-B759-FC80F0204251}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8ECC3293-1372-455C-AD0A-D32453F3236D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
   </bookViews>
   <sheets>
     <sheet name="iCC390" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'iCC390'!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iCC464'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'iCC644'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'iCC644'!$A$1:$A$136</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="3">'iCC644'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="214">
   <si>
     <t>exchange</t>
   </si>
@@ -690,8 +691,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -719,9 +728,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22685EC5-16DE-4AFB-A090-DFD06D9263EB}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection sqref="A1:B77"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1106,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B7">
@@ -1396,7 +1406,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B42">
@@ -1492,7 +1502,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B54">
@@ -1500,7 +1510,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B55">
@@ -1572,7 +1582,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B64">
@@ -1612,7 +1622,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="A69" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B69">
@@ -1620,7 +1630,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="A70" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B70">
@@ -1628,7 +1638,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B71">
@@ -1685,6 +1695,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1692,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F2E160-0E44-4C80-A334-F20DED143A47}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A43"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2058,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44">
@@ -2079,7 +2090,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48">
@@ -2159,7 +2170,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B58">
@@ -2255,7 +2266,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B70">
@@ -2263,7 +2274,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B71">
@@ -2279,7 +2290,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B73">
@@ -2319,7 +2330,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B78">
@@ -2327,7 +2338,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B79">
@@ -2335,7 +2346,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B80">
@@ -2343,7 +2354,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B81">
@@ -2351,7 +2362,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B82">
@@ -2824,7 +2835,7 @@
   <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2921,7 +2932,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B12">
@@ -3169,7 +3180,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B43">
@@ -3225,7 +3236,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B50">
@@ -3249,7 +3260,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B53">
@@ -3401,7 +3412,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="A72" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B72">
@@ -3409,7 +3420,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="A73" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B73">
@@ -3489,7 +3500,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="A83" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B83">
@@ -3569,7 +3580,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="A93" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B93">
@@ -3679,10 +3690,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02346A24-1580-4C64-B8C8-03FE59A3BFAA}">
-  <dimension ref="A1:B138"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection sqref="A1:B138"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3699,8 +3710,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
+      <c r="A2" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B2">
         <v>999999</v>
@@ -3708,7 +3719,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>999999</v>
@@ -3716,7 +3727,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>999999</v>
@@ -3724,7 +3735,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="B5">
         <v>999999</v>
@@ -3732,7 +3743,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>999999</v>
@@ -3740,7 +3751,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>999999</v>
@@ -3748,7 +3759,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>999999</v>
@@ -3756,7 +3767,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>999999</v>
@@ -3764,7 +3775,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="B10">
         <v>999999</v>
@@ -3772,7 +3783,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>999999</v>
@@ -3780,7 +3791,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>999999</v>
@@ -3788,7 +3799,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>999999</v>
@@ -3796,7 +3807,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>999999</v>
@@ -3804,7 +3815,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>999999</v>
@@ -3812,7 +3823,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>999999</v>
@@ -3820,7 +3831,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="B17">
         <v>999999</v>
@@ -3828,7 +3839,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>999999</v>
@@ -3844,7 +3855,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3852,7 +3863,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3860,7 +3871,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3868,7 +3879,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3876,7 +3887,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3884,7 +3895,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3892,7 +3903,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3900,7 +3911,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3908,7 +3919,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3916,7 +3927,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3924,7 +3935,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3932,7 +3943,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3940,7 +3951,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3948,7 +3959,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3956,7 +3967,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3964,7 +3975,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -3972,7 +3983,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3980,7 +3991,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3988,7 +3999,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4004,7 +4015,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -4012,7 +4023,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -4020,7 +4031,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4028,7 +4039,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -4036,7 +4047,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -4044,7 +4055,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -4052,15 +4063,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>186</v>
+      <c r="A47" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -4068,7 +4079,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>168</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -4076,15 +4087,15 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>70</v>
+      <c r="A50" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -4092,7 +4103,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>89</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4100,7 +4111,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -4108,7 +4119,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -4116,7 +4127,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4124,7 +4135,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4132,7 +4143,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>203</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -4140,7 +4151,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -4148,7 +4159,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4156,7 +4167,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>204</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -4164,7 +4175,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>183</v>
+        <v>111</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4172,7 +4183,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -4180,7 +4191,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -4188,7 +4199,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>213</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -4196,23 +4207,23 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>175</v>
+      <c r="A65" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>77</v>
+      <c r="A66" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -4220,7 +4231,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -4228,7 +4239,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -4236,7 +4247,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>179</v>
+        <v>96</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -4244,7 +4255,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>106</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -4252,7 +4263,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -4260,15 +4271,15 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>50</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>156</v>
+      <c r="A73" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -4276,7 +4287,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -4284,15 +4295,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>86</v>
+      <c r="A76" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -4300,15 +4311,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>205</v>
+      <c r="A78" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -4316,7 +4327,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>192</v>
+        <v>61</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -4324,15 +4335,15 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>212</v>
+      <c r="A81" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -4340,7 +4351,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -4348,7 +4359,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>210</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -4356,7 +4367,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>200</v>
+        <v>54</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -4364,7 +4375,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -4372,7 +4383,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -4380,7 +4391,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>192</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -4388,7 +4399,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -4396,7 +4407,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -4404,7 +4415,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -4412,7 +4423,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -4420,7 +4431,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -4428,7 +4439,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -4436,7 +4447,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -4444,7 +4455,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -4452,7 +4463,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -4460,7 +4471,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -4468,7 +4479,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -4476,7 +4487,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>201</v>
+        <v>84</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4484,7 +4495,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>208</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -4492,31 +4503,31 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>88</v>
+      <c r="A102" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>195</v>
+      <c r="A103" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>142</v>
+      <c r="A104" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -4524,7 +4535,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -4532,7 +4543,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -4540,7 +4551,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -4548,7 +4559,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -4556,7 +4567,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -4564,7 +4575,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -4572,7 +4583,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -4580,7 +4591,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -4588,7 +4599,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -4596,7 +4607,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -4604,7 +4615,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -4612,7 +4623,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>207</v>
+        <v>139</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -4620,7 +4631,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
+        <v>159</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -4628,7 +4639,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>213</v>
+        <v>132</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -4636,7 +4647,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -4644,7 +4655,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>61</v>
+        <v>175</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -4652,7 +4663,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -4660,7 +4671,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -4668,7 +4679,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -4676,7 +4687,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -4684,7 +4695,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -4692,7 +4703,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -4700,15 +4711,15 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="B127">
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>69</v>
+      <c r="A128" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -4716,7 +4727,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>185</v>
+        <v>45</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -4724,7 +4735,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -4732,7 +4743,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>197</v>
+        <v>144</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -4740,7 +4751,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -4748,7 +4759,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -4756,7 +4767,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -4764,7 +4775,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>198</v>
+        <v>18</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -4772,29 +4783,16 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
       <c r="B136">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>43</v>
-      </c>
-      <c r="B137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>54</v>
-      </c>
-      <c r="B138">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B139">
+    <sortCondition descending="1" ref="B1:B139"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>